<commit_message>
made: graph of COVIDs lockdown measures for top 5 countries with statistical analysis, calculated share of total ghg from the 5 countries, showed per unit energy emissions of the selected countries with statistical analysis. Making a workflowset now
</commit_message>
<xml_diff>
--- a/data/Gov_Responses_Sources.xlsx
+++ b/data/Gov_Responses_Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua Puyear\Documents\csu-undergrad\ess-330-joshp-2025\github\ESS-330-FinalProject-April23\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0BCF51-E77A-471D-B593-0860AC1EA981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F190B8-F051-4518-AE41-199187571C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="17280" windowHeight="12336" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -4128,12 +4128,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.3984375" customWidth="1"/>
-    <col min="6" max="6" width="59.8984375" customWidth="1"/>
+    <col min="1" max="1" width="133.69921875" customWidth="1"/>
+    <col min="2" max="4" width="9.3984375" customWidth="1"/>
+    <col min="5" max="5" width="96.8984375" customWidth="1"/>
+    <col min="6" max="6" width="76.59765625" customWidth="1"/>
     <col min="7" max="26" width="9.3984375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5136,8 +5138,8 @@
     <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14548,7 +14550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>